<commit_message>
There was an incorrect year in the tucp file
</commit_message>
<xml_diff>
--- a/data/tucp_dates.xlsx
+++ b/data/tucp_dates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://doimspp-my.sharepoint.com/personal/cpien_usbr_gov/Documents/Work/HAB/EDB-HABs-Weeds/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{0CE30478-94AB-45AC-809E-46FA8F1BE5B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AC01E2D3-1A9D-4CA2-A605-1E64021317D3}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{0CE30478-94AB-45AC-809E-46FA8F1BE5B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{31900CD7-3FB0-4D3A-8CAE-00989C9B923A}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{64D01899-1BFE-4765-BDEF-172C7691D551}"/>
+    <workbookView xWindow="10" yWindow="0" windowWidth="19180" windowHeight="10200" xr2:uid="{64D01899-1BFE-4765-BDEF-172C7691D551}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -440,20 +440,20 @@
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="16.42578125" customWidth="1"/>
+    <col min="2" max="2" width="16.453125" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="5" max="5" width="14.85546875" customWidth="1"/>
-    <col min="6" max="6" width="14.7109375" customWidth="1"/>
-    <col min="8" max="8" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.42578125" customWidth="1"/>
+    <col min="5" max="5" width="14.81640625" customWidth="1"/>
+    <col min="6" max="6" width="14.7265625" customWidth="1"/>
+    <col min="8" max="8" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -485,7 +485,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>2011</v>
       </c>
@@ -496,7 +496,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2012</v>
       </c>
@@ -507,7 +507,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>2013</v>
       </c>
@@ -518,7 +518,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>2014</v>
       </c>
@@ -541,7 +541,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>2015</v>
       </c>
@@ -570,7 +570,7 @@
         <v>42095</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>2016</v>
       </c>
@@ -581,7 +581,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>2017</v>
       </c>
@@ -592,7 +592,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>2018</v>
       </c>
@@ -603,7 +603,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>2019</v>
       </c>
@@ -614,7 +614,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>2020</v>
       </c>
@@ -625,7 +625,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>2021</v>
       </c>
@@ -642,7 +642,7 @@
         <v>44369</v>
       </c>
       <c r="F12" s="1">
-        <v>44944</v>
+        <v>44579</v>
       </c>
       <c r="G12" t="s">
         <v>14</v>
@@ -657,7 +657,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>2022</v>
       </c>

</xml_diff>